<commit_message>
feat: edit docs and excel
Edit manual test detail and tracbility matrix based on Punnut and Pongkrit.
</commit_message>
<xml_diff>
--- a/manual test cases/traceability matrix.xlsx
+++ b/manual test cases/traceability matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silsl\Documents\GitHub\SAATM\manual test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085ACB59-D822-4BBF-8863-3D5C58B0233C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B988C37F-29E5-4594-98ED-1A77246E0DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6C1DD0C9-4242-4CB0-B375-6B3E62372787}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>SAATM-3-1</t>
   </si>
   <si>
-    <t>SAATM-3-2</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -125,36 +122,12 @@
     <t>Test whether our software can handle searches by type flight number that does not exist in the system right now.</t>
   </si>
   <si>
-    <t>Test whether our software can filter flight altitude from 1000 ft. to 16000 ft.</t>
-  </si>
-  <si>
-    <t>Flight’s altitude 1000 – 16000 ft. filtering test.</t>
-  </si>
-  <si>
-    <t>Test whether our software can filter flight altitudes at more than 16000 feet.</t>
-  </si>
-  <si>
-    <t>Test whether our software can filter flight altitude at less than 2000 ft.</t>
-  </si>
-  <si>
-    <t>Hide info boxes.</t>
-  </si>
-  <si>
-    <t>Test whether our software can hide the info boxes.</t>
-  </si>
-  <si>
     <t>Show info boxes.</t>
   </si>
   <si>
     <t>Test whether our software can show the info boxes.</t>
   </si>
   <si>
-    <t xml:space="preserve">Flight’s altitude &gt; 16000 filtering test. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flight’s altitude &lt; 2000 ft. filtering test. </t>
-  </si>
-  <si>
     <t>Search Flight by flight number</t>
   </si>
   <si>
@@ -171,6 +144,33 @@
   </si>
   <si>
     <t>Allow user to hide or show info boxes.</t>
+  </si>
+  <si>
+    <t>SAATM-2-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight’s altitude 0 – 16000 ft. filtering test. </t>
+  </si>
+  <si>
+    <t>Test whether our software can filter flight altitude from 0 ft. to 16000 ft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight's minimum altitude filtering test (10000 ft)  </t>
+  </si>
+  <si>
+    <t>Test whether our software can filter flights by minimum altitude of 10000 ft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight's maximum altitude filtering test (16000 ft)  </t>
+  </si>
+  <si>
+    <t>Test whether our software can filter flights by maximum altitude of 16000 ft.</t>
+  </si>
+  <si>
+    <t>Clear all altitude filters test</t>
+  </si>
+  <si>
+    <t>Test whether our software can clear all altitude filters and show all flights.</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,54 +636,54 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -691,93 +691,93 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>